<commit_message>
...idk, too much thing i do...
</commit_message>
<xml_diff>
--- a/ExportExcel/DanhSachSinhVien.xlsx
+++ b/ExportExcel/DanhSachSinhVien.xlsx
@@ -34,49 +34,22 @@
     <x:t>QueQuan</x:t>
   </x:si>
   <x:si>
-    <x:t>73DCHT22204</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HT001</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Đinh Đức Giang</x:t>
+    <x:t>qwe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nguyễn Văn A</x:t>
   </x:si>
   <x:si>
     <x:t>Nam</x:t>
   </x:si>
   <x:si>
-    <x:t>1/29/2004 12:00:00 AM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Quảng Ninh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SV001</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nguyễn Văn A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1/1/2000 12:00:00 AM</x:t>
+    <x:t>5/15/2000 12:00:00 AM</x:t>
   </x:si>
   <x:si>
     <x:t>Hà Nội</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SV002</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trần Thị B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nữ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3/15/2001 12:00:00 AM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TP. HCM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -140,8 +113,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0">
-  <x:autoFilter ref="A1:F4"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F2" totalsRowShown="0">
+  <x:autoFilter ref="A1:F2"/>
   <x:tableColumns count="6">
     <x:tableColumn id="1" name="MaSinhVien"/>
     <x:tableColumn id="2" name="Malop"/>
@@ -442,7 +415,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F4"/>
+  <x:dimension ref="A1:F2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -486,46 +459,6 @@
       </x:c>
       <x:c r="F2" s="0" t="s">
         <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:6">
-      <x:c r="A3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6">
-      <x:c r="A4" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>20</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>